<commit_message>
Vanilla Furniture Expanded - Spacer Module 번역 갱신 & 1.6 폴더 추가
</commit_message>
<xml_diff>
--- a/Data/Vanilla Expanded/Vanilla Furniture Expanded - Spacer Module - 2028381079/1.5/2028381079.xlsx
+++ b/Data/Vanilla Expanded/Vanilla Furniture Expanded - Spacer Module - 2028381079/1.5/2028381079.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SteamLibrary\steamapps\common\RimWorld\Mods\rk_tran\Data\Vanilla Furniture Expanded - Spacer Module - 2028381079\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SteamLibrary\steamapps\common\RimWorld\Mods\RMK\Data\Vanilla Expanded\Vanilla Furniture Expanded - Spacer Module - 2028381079\1.5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D418133-1837-477C-B85D-996587CAAB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7CA1C7-0C1B-43BA-AB6F-97B659D6C1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="308">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -786,6 +799,168 @@
   </si>
   <si>
     <t>여기 저장된 무기와 의상은 HP가 완전히 회복될 때까지 자동으로 사용 금지됩니다</t>
+  </si>
+  <si>
+    <t>ThingDef+VFES_Table_IlluminatedWardrobe.label</t>
+  </si>
+  <si>
+    <t>VFES_Table_IlluminatedWardrobe.label</t>
+  </si>
+  <si>
+    <t>조명 대형 옷장</t>
+  </si>
+  <si>
+    <t>ThingDef+VFES_Table_IlluminatedWardrobe.description</t>
+  </si>
+  <si>
+    <t>VFES_Table_IlluminatedWardrobe.description</t>
+  </si>
+  <si>
+    <t>부드럽게 빛나는 조명이 내장된 세련된 현대식 옷장입니다. 주변 침대의 편안함과 수면 효율을 약간 올려줍니다. 같은 침대 근처에 여러 개를 두어도 효과는 중첩되지 않습니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+VFES_WallMountedTelevision.label</t>
+  </si>
+  <si>
+    <t>VFES_WallMountedTelevision.label</t>
+  </si>
+  <si>
+    <t>벽걸이 TV</t>
+  </si>
+  <si>
+    <t>ThingDef+VFES_WallMountedTelevision.description</t>
+  </si>
+  <si>
+    <t>VFES_WallMountedTelevision.description</t>
+  </si>
+  <si>
+    <t>얇은 고성능 평면 TV입니다. 공간을 적게 차지하면서도 일반 평면 TV와 동급의 선명한 화질과 색감을 제공합니다. 시야각은 넓지 않지만 벽에 설치할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+VFES_TelevisionSpeaker.label</t>
+  </si>
+  <si>
+    <t>VFES_TelevisionSpeaker.label</t>
+  </si>
+  <si>
+    <t>TV 스피커</t>
+  </si>
+  <si>
+    <t>ThingDef+VFES_TelevisionSpeaker.description</t>
+  </si>
+  <si>
+    <t>VFES_TelevisionSpeaker.description</t>
+  </si>
+  <si>
+    <t>TV 시청 경험을 향상시키기 위해 설계된 고음질 오디오 시스템입니다. TV 근처에 배치하면 자동으로 연동되어 몰입감 있는 사운드를 제공하며, 시청 중인 정착민의 오락 욕구 충족도를 높입니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Spacer_OutdoorLamp.comps.3.offMessage</t>
+  </si>
+  <si>
+    <t>Spacer_OutdoorLamp.comps.3.offMessage</t>
+  </si>
+  <si>
+    <t>전원 꺼짐: 충분한 햇빛 있음</t>
+  </si>
+  <si>
+    <t>ThingDef+VFES_AirPurifier.label</t>
+  </si>
+  <si>
+    <t>VFES_AirPurifier.label</t>
+  </si>
+  <si>
+    <t>공기 청정기</t>
+  </si>
+  <si>
+    <t>ThingDef+VFES_AirPurifier.description</t>
+  </si>
+  <si>
+    <t>VFES_AirPurifier.description</t>
+  </si>
+  <si>
+    <t>작고 효율적인 공기 청정기로, 먼지, 알레르기 유발 물질, 연기 등 유해 물질을 걸러내며 향기로운 공기를 순환시킵니다. 방의 청결도를 높이고 기분을 약간 향상시키며, 전반적인 환경을 개선합니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+VFES_ModernArmchair.label</t>
+  </si>
+  <si>
+    <t>VFES_ModernArmchair.label</t>
+  </si>
+  <si>
+    <t>현대식 팔걸이 의자</t>
+  </si>
+  <si>
+    <t>ThingDef+VFES_ModernArmchair.description</t>
+  </si>
+  <si>
+    <t>VFES_ModernArmchair.description</t>
+  </si>
+  <si>
+    <t>우주 시대의 세련된 팔걸이 의자입니다. 메모리폼과 스마트 천으로 만들어졌으며 인체공학적 설계로 뛰어난 편안함과 미적 만족을 제공합니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+VFES_ModernCouch.label</t>
+  </si>
+  <si>
+    <t>VFES_ModernCouch.label</t>
+  </si>
+  <si>
+    <t>현대식 카우치</t>
+  </si>
+  <si>
+    <t>ThingDef+VFES_ModernCouch.description</t>
+  </si>
+  <si>
+    <t>VFES_ModernCouch.description</t>
+  </si>
+  <si>
+    <t>우주 시대의 세련된 2인용 카우치입니다. 메모리폼과 인체공학적 설계, 스마트 천 덕에 최고의 편안함을 제공합니다.</t>
+  </si>
+  <si>
+    <t>ThoughtDef+VFES_FreshAir.stages.0.label</t>
+  </si>
+  <si>
+    <t>ThoughtDef</t>
+  </si>
+  <si>
+    <t>VFES_FreshAir.stages.0.label</t>
+  </si>
+  <si>
+    <t>상쾌한 공기</t>
+  </si>
+  <si>
+    <t>ThoughtDef+VFES_FreshAir.stages.0.description</t>
+  </si>
+  <si>
+    <t>VFES_FreshAir.stages.0.description</t>
+  </si>
+  <si>
+    <t>산뜻한 향이 나는 상쾌한 공기를 마셨어!</t>
+  </si>
+  <si>
+    <t>HediffDef+VFES_FreshAir.label</t>
+  </si>
+  <si>
+    <t>VFES_FreshAir.label</t>
+  </si>
+  <si>
+    <t>HediffDef+VFES_FreshAir.description</t>
+  </si>
+  <si>
+    <t>VFES_FreshAir.description</t>
+  </si>
+  <si>
+    <t>JobDef+VFES_UseInteractiveTable.reportString</t>
+  </si>
+  <si>
+    <t>JobDef</t>
+  </si>
+  <si>
+    <t>VFES_UseInteractiveTable.reportString</t>
+  </si>
+  <si>
+    <t>대화식 탁자 사용 중.</t>
   </si>
 </sst>
 </file>
@@ -1149,10 +1324,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="K83" sqref="K83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2221,6 +2396,258 @@
         <v>253</v>
       </c>
     </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>